<commit_message>
Slightly improved project structure
</commit_message>
<xml_diff>
--- a/data/starters.xlsx
+++ b/data/starters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\PyProjects\Bots\violetsbot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\PyProjects\Bots\NewVioletsBot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB0CCBA2-C6F2-42DB-81EE-0D7E0083D7BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF33E61A-9D6D-4BE2-9B57-8C97399BD78C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2103,9 +2103,6 @@
     <t>ЕК - Хрустальные росы</t>
   </si>
   <si>
-    <t>Zipper Zapper</t>
-  </si>
-  <si>
     <t>Buckeye Irish Lace</t>
   </si>
   <si>
@@ -2386,6 +2383,9 @@
   </si>
   <si>
     <t>Ящик #15</t>
+  </si>
+  <si>
+    <t>Rob's Zipper Zapper</t>
   </si>
 </sst>
 </file>
@@ -2594,19 +2594,19 @@
     <tableColumn id="31" xr3:uid="{9A3134C2-FCCA-4BB8-A528-3912CF378C66}" name="Ящик #9" dataDxfId="15"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Ящик #10" dataDxfId="14"/>
     <tableColumn id="22" xr3:uid="{6197D5A9-F618-41B3-A889-CF2C90B91E32}" name="Ящик #12" dataDxfId="13"/>
-    <tableColumn id="28" xr3:uid="{EF374C7C-8111-4C0E-9EC6-5D2F8CBEEABA}" name="Ящик #15" dataDxfId="0"/>
-    <tableColumn id="30" xr3:uid="{DA8250A9-98B2-42F0-B04F-8689E21D3BA3}" name="Ящик #16" dataDxfId="12"/>
-    <tableColumn id="18" xr3:uid="{D368CEA8-420E-4BEF-BE16-8A1005E7C127}" name="Ящик #17" dataDxfId="11"/>
-    <tableColumn id="20" xr3:uid="{4B147DB0-97D4-4554-B343-12ADD677FA7F}" name="Ящик #18" dataDxfId="10"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Ящик #19" dataDxfId="9"/>
-    <tableColumn id="14" xr3:uid="{D78ABCB0-302A-4254-999B-1FC54CBFF846}" name="Ящик #20" dataDxfId="8"/>
-    <tableColumn id="19" xr3:uid="{7EBC64F3-C900-44F2-9A91-31C419C32BE0}" name="Ящик #22" dataDxfId="7"/>
-    <tableColumn id="12" xr3:uid="{FA5F0F81-CB90-4BA6-918B-2B52D493837B}" name="Ящик #23" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{98A2E7B9-0D47-42A6-8901-D2512ABD6BC2}" name="Ящик #24 (взр)" dataDxfId="5"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Ящик #25" dataDxfId="4"/>
-    <tableColumn id="15" xr3:uid="{E359A471-57FE-447B-9F03-1D112E97414A}" name="Ящик #26" dataDxfId="3"/>
-    <tableColumn id="25" xr3:uid="{8497A312-7E4D-49CF-8F2A-4386289CF750}" name="Лоток #43" dataDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{ED14E19E-75E7-4626-9AE4-D2D302EB8DE8}" name="Лоток желтый" dataDxfId="1"/>
+    <tableColumn id="28" xr3:uid="{EF374C7C-8111-4C0E-9EC6-5D2F8CBEEABA}" name="Ящик #15" dataDxfId="12"/>
+    <tableColumn id="30" xr3:uid="{DA8250A9-98B2-42F0-B04F-8689E21D3BA3}" name="Ящик #16" dataDxfId="11"/>
+    <tableColumn id="18" xr3:uid="{D368CEA8-420E-4BEF-BE16-8A1005E7C127}" name="Ящик #17" dataDxfId="10"/>
+    <tableColumn id="20" xr3:uid="{4B147DB0-97D4-4554-B343-12ADD677FA7F}" name="Ящик #18" dataDxfId="9"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Ящик #19" dataDxfId="8"/>
+    <tableColumn id="14" xr3:uid="{D78ABCB0-302A-4254-999B-1FC54CBFF846}" name="Ящик #20" dataDxfId="7"/>
+    <tableColumn id="19" xr3:uid="{7EBC64F3-C900-44F2-9A91-31C419C32BE0}" name="Ящик #22" dataDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{FA5F0F81-CB90-4BA6-918B-2B52D493837B}" name="Ящик #23" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{98A2E7B9-0D47-42A6-8901-D2512ABD6BC2}" name="Ящик #24 (взр)" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Ящик #25" dataDxfId="3"/>
+    <tableColumn id="15" xr3:uid="{E359A471-57FE-447B-9F03-1D112E97414A}" name="Ящик #26" dataDxfId="2"/>
+    <tableColumn id="25" xr3:uid="{8497A312-7E4D-49CF-8F2A-4386289CF750}" name="Лоток #43" dataDxfId="1"/>
+    <tableColumn id="16" xr3:uid="{ED14E19E-75E7-4626-9AE4-D2D302EB8DE8}" name="Лоток желтый" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2912,8 +2912,8 @@
   <dimension ref="A1:AF756"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A500" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C507" sqref="C507"/>
+      <pane ySplit="1" topLeftCell="A590" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C603" sqref="C603"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2952,7 +2952,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -2982,13 +2982,13 @@
         <v>644</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>498</v>
@@ -2997,7 +2997,7 @@
         <v>4</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>5</v>
@@ -3006,10 +3006,10 @@
         <v>565</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>496</v>
@@ -3030,24 +3030,24 @@
         <v>564</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="AC1" s="1" t="s">
         <v>9</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="AE1" s="1" t="s">
         <v>636</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -3145,7 +3145,7 @@
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="B3" s="4">
         <v>1</v>
@@ -3243,7 +3243,7 @@
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B4" s="4">
         <v>0</v>
@@ -3341,7 +3341,7 @@
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="B5" s="4">
         <v>0</v>
@@ -3537,7 +3537,7 @@
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="B7" s="4">
         <v>0</v>
@@ -3929,7 +3929,7 @@
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="B11" s="4">
         <v>0</v>
@@ -5693,7 +5693,7 @@
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B29" s="4">
         <v>1</v>
@@ -6575,7 +6575,7 @@
     </row>
     <row r="38" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="B38" s="4">
         <v>1</v>
@@ -7469,7 +7469,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F47" s="4">
         <v>0</v>
@@ -8927,7 +8927,7 @@
     </row>
     <row r="62" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B62" s="4">
         <v>0</v>
@@ -12455,7 +12455,7 @@
     </row>
     <row r="98" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A98" s="2" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B98" s="4">
         <v>1</v>
@@ -12553,7 +12553,7 @@
     </row>
     <row r="99" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A99" s="2" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="B99" s="4">
         <v>0</v>
@@ -12651,7 +12651,7 @@
     </row>
     <row r="100" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A100" s="2" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="B100" s="4">
         <v>0</v>
@@ -14611,7 +14611,7 @@
     </row>
     <row r="120" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A120" s="2" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="B120" s="4">
         <v>0</v>
@@ -14763,7 +14763,7 @@
         <v>0</v>
       </c>
       <c r="S121" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T121" s="4">
         <v>0</v>
@@ -15395,7 +15395,7 @@
     </row>
     <row r="128" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A128" s="2" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="B128" s="4">
         <v>0</v>
@@ -15787,7 +15787,7 @@
     </row>
     <row r="132" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B132" s="4">
         <v>0</v>
@@ -17159,7 +17159,7 @@
     </row>
     <row r="146" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A146" s="2" t="s">
-        <v>692</v>
+        <v>786</v>
       </c>
       <c r="B146" s="4">
         <v>0</v>
@@ -17257,7 +17257,7 @@
     </row>
     <row r="147" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A147" s="2" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="B147" s="4">
         <v>0</v>
@@ -17801,7 +17801,7 @@
         <v>0</v>
       </c>
       <c r="S152" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T152" s="4">
         <v>0</v>
@@ -18083,7 +18083,7 @@
         <v>0</v>
       </c>
       <c r="O155" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P155" s="4">
         <v>0</v>
@@ -18531,7 +18531,7 @@
     </row>
     <row r="160" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A160" s="2" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="B160" s="4">
         <v>0</v>
@@ -19315,7 +19315,7 @@
     </row>
     <row r="168" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A168" s="2" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="B168" s="4">
         <v>0</v>
@@ -19511,7 +19511,7 @@
     </row>
     <row r="170" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A170" s="2" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="B170" s="4">
         <v>0</v>
@@ -19912,7 +19912,7 @@
         <v>0</v>
       </c>
       <c r="D174" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E174" s="4">
         <v>0</v>
@@ -21177,7 +21177,7 @@
     </row>
     <row r="187" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A187" s="2" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="B187" s="4">
         <v>1</v>
@@ -22157,7 +22157,7 @@
     </row>
     <row r="197" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A197" s="2" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="B197" s="4">
         <v>0</v>
@@ -22353,7 +22353,7 @@
     </row>
     <row r="199" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A199" s="2" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B199" s="4">
         <v>0</v>
@@ -23235,7 +23235,7 @@
     </row>
     <row r="208" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A208" s="2" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="B208" s="4">
         <v>0</v>
@@ -24215,7 +24215,7 @@
     </row>
     <row r="218" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A218" s="2" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="B218" s="4">
         <v>0</v>
@@ -24509,7 +24509,7 @@
     </row>
     <row r="221" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A221" s="2" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="B221" s="4">
         <v>1</v>
@@ -24803,7 +24803,7 @@
     </row>
     <row r="224" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A224" s="2" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="B224" s="4">
         <v>0</v>
@@ -24901,7 +24901,7 @@
     </row>
     <row r="225" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A225" s="2" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="B225" s="4">
         <v>0</v>
@@ -24999,7 +24999,7 @@
     </row>
     <row r="226" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A226" s="2" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="B226" s="4">
         <v>0</v>
@@ -25391,7 +25391,7 @@
     </row>
     <row r="230" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A230" s="2" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="B230" s="4">
         <v>0</v>
@@ -27253,7 +27253,7 @@
     </row>
     <row r="249" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A249" s="2" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="B249" s="4">
         <v>1</v>
@@ -27351,7 +27351,7 @@
     </row>
     <row r="250" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A250" s="2" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="B250" s="4">
         <v>0</v>
@@ -27411,7 +27411,7 @@
         <v>0</v>
       </c>
       <c r="U250" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V250" s="4">
         <v>0</v>
@@ -27841,7 +27841,7 @@
     </row>
     <row r="255" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A255" s="2" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="B255" s="4">
         <v>0</v>
@@ -28527,7 +28527,7 @@
     </row>
     <row r="262" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A262" s="2" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="B262" s="4">
         <v>1</v>
@@ -29801,7 +29801,7 @@
     </row>
     <row r="275" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A275" s="2" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B275" s="4">
         <v>0</v>
@@ -29899,7 +29899,7 @@
     </row>
     <row r="276" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A276" s="2" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="B276" s="4">
         <v>0</v>
@@ -32055,7 +32055,7 @@
     </row>
     <row r="298" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A298" s="2" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="B298" s="4">
         <v>0</v>
@@ -32545,7 +32545,7 @@
     </row>
     <row r="303" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A303" s="2" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="B303" s="4">
         <v>0</v>
@@ -33623,7 +33623,7 @@
     </row>
     <row r="314" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A314" s="2" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="B314" s="4">
         <v>0</v>
@@ -34113,7 +34113,7 @@
     </row>
     <row r="319" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A319" s="2" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="B319" s="4">
         <v>0</v>
@@ -34995,7 +34995,7 @@
     </row>
     <row r="328" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A328" s="2" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="B328" s="4">
         <v>0</v>
@@ -35289,7 +35289,7 @@
     </row>
     <row r="331" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A331" s="2" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="B331" s="4">
         <v>0</v>
@@ -36759,7 +36759,7 @@
     </row>
     <row r="346" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A346" s="2" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="B346" s="4">
         <v>0</v>
@@ -37009,7 +37009,7 @@
         <v>0</v>
       </c>
       <c r="S348" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T348" s="4">
         <v>0</v>
@@ -37543,7 +37543,7 @@
     </row>
     <row r="354" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A354" s="2" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="B354" s="4">
         <v>0</v>
@@ -38327,7 +38327,7 @@
     </row>
     <row r="362" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A362" s="2" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="B362" s="4">
         <v>0</v>
@@ -39111,7 +39111,7 @@
     </row>
     <row r="370" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A370" s="2" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="B370" s="4">
         <v>0</v>
@@ -39601,7 +39601,7 @@
     </row>
     <row r="375" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A375" s="2" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="B375" s="4">
         <v>1</v>
@@ -42497,7 +42497,7 @@
         <v>0</v>
       </c>
       <c r="S404" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T404" s="4">
         <v>0</v>
@@ -42639,7 +42639,7 @@
     </row>
     <row r="406" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A406" s="2" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="B406" s="4">
         <v>0</v>
@@ -46265,7 +46265,7 @@
     </row>
     <row r="443" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A443" s="2" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B443" s="4">
         <v>0</v>
@@ -46559,7 +46559,7 @@
     </row>
     <row r="446" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A446" s="2" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="B446" s="4">
         <v>0</v>
@@ -46755,7 +46755,7 @@
     </row>
     <row r="448" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A448" s="2" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="B448" s="4">
         <v>0</v>
@@ -48225,7 +48225,7 @@
     </row>
     <row r="463" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A463" s="2" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B463" s="4">
         <v>0</v>
@@ -49250,7 +49250,7 @@
         <v>0</v>
       </c>
       <c r="P473" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q473" s="4">
         <v>0</v>
@@ -49446,7 +49446,7 @@
         <v>0</v>
       </c>
       <c r="P475" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q475" s="4">
         <v>0</v>
@@ -51513,7 +51513,7 @@
         <v>0</v>
       </c>
       <c r="S496" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T496" s="4">
         <v>0</v>
@@ -51753,7 +51753,7 @@
     </row>
     <row r="499" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A499" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="B499" s="4">
         <v>0</v>
@@ -52635,7 +52635,7 @@
     </row>
     <row r="508" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A508" s="2" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="B508" s="4">
         <v>1</v>
@@ -53909,7 +53909,7 @@
     </row>
     <row r="521" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A521" s="2" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B521" s="4">
         <v>0</v>
@@ -54791,7 +54791,7 @@
     </row>
     <row r="530" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A530" s="2" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="B530" s="4">
         <v>0</v>
@@ -54889,7 +54889,7 @@
     </row>
     <row r="531" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A531" s="2" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="B531" s="4">
         <v>0</v>
@@ -55575,7 +55575,7 @@
     </row>
     <row r="538" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A538" s="2" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="B538" s="4">
         <v>0</v>
@@ -56065,7 +56065,7 @@
     </row>
     <row r="543" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A543" s="2" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="B543" s="4">
         <v>0</v>
@@ -56947,10 +56947,10 @@
     </row>
     <row r="552" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A552" s="2" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="B552" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C552" s="4">
         <v>0</v>
@@ -57143,7 +57143,7 @@
     </row>
     <row r="554" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A554" s="2" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="B554" s="4">
         <v>0</v>
@@ -57241,7 +57241,7 @@
     </row>
     <row r="555" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A555" s="2" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="B555" s="4">
         <v>1</v>
@@ -57437,7 +57437,7 @@
     </row>
     <row r="557" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A557" s="2" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B557" s="4">
         <v>0</v>
@@ -59005,7 +59005,7 @@
     </row>
     <row r="573" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A573" s="2" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="B573" s="4">
         <v>0</v>
@@ -59397,7 +59397,7 @@
     </row>
     <row r="577" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A577" s="2" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B577" s="4">
         <v>0</v>
@@ -59593,7 +59593,7 @@
     </row>
     <row r="579" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A579" s="2" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="B579" s="4">
         <v>0</v>
@@ -59691,7 +59691,7 @@
     </row>
     <row r="580" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A580" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="B580" s="4">
         <v>0</v>
@@ -60247,7 +60247,7 @@
         <v>0</v>
       </c>
       <c r="W585" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X585" s="4">
         <v>0</v>
@@ -60377,7 +60377,7 @@
     </row>
     <row r="587" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A587" s="2" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="B587" s="4">
         <v>0</v>
@@ -61161,7 +61161,7 @@
     </row>
     <row r="595" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A595" s="2" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="B595" s="4">
         <v>0</v>
@@ -61847,7 +61847,7 @@
     </row>
     <row r="602" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A602" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="B602" s="4">
         <v>0</v>
@@ -62337,7 +62337,7 @@
     </row>
     <row r="607" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A607" s="2" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="B607" s="4">
         <v>0</v>
@@ -62435,7 +62435,7 @@
     </row>
     <row r="608" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A608" s="2" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="B608" s="4">
         <v>0</v>
@@ -64787,7 +64787,7 @@
     </row>
     <row r="632" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A632" s="2" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="B632" s="4">
         <v>0</v>
@@ -66257,7 +66257,7 @@
     </row>
     <row r="647" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A647" s="2" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B647" s="4">
         <v>0</v>
@@ -66943,7 +66943,7 @@
     </row>
     <row r="654" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A654" s="2" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B654" s="4">
         <v>0</v>
@@ -67825,7 +67825,7 @@
     </row>
     <row r="663" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A663" s="2" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="B663" s="4">
         <v>1</v>
@@ -69001,7 +69001,7 @@
     </row>
     <row r="675" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A675" s="2" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="B675" s="4">
         <v>0</v>
@@ -69687,7 +69687,7 @@
     </row>
     <row r="682" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A682" s="2" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="B682" s="4">
         <v>0</v>
@@ -70177,7 +70177,7 @@
     </row>
     <row r="687" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A687" s="2" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="B687" s="4">
         <v>0</v>
@@ -70667,7 +70667,7 @@
     </row>
     <row r="692" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A692" s="2" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="B692" s="4">
         <v>0</v>
@@ -71941,7 +71941,7 @@
     </row>
     <row r="705" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A705" s="2" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B705" s="4">
         <v>1</v>
@@ -72333,7 +72333,7 @@
     </row>
     <row r="709" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A709" s="2" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B709" s="4">
         <v>0</v>
@@ -73866,7 +73866,7 @@
         <v>0</v>
       </c>
       <c r="V724" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W724" s="4">
         <v>0</v>
@@ -73999,7 +73999,7 @@
     </row>
     <row r="726" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A726" s="2" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="B726" s="4">
         <v>0</v>
@@ -74881,7 +74881,7 @@
     </row>
     <row r="735" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A735" s="2" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="B735" s="4">
         <v>0</v>
@@ -76209,7 +76209,7 @@
         <v>0</v>
       </c>
       <c r="S748" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T748" s="4">
         <v>0</v>
@@ -76253,7 +76253,7 @@
     </row>
     <row r="749" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A749" s="2" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="B749" s="4">
         <v>0</v>

</xml_diff>